<commit_message>
get all, get by id toeic_test endpoint
</commit_message>
<xml_diff>
--- a/back-end/uploads/TEST 1 - ETS 2024/TEST 1 - ETS 2024-PASSAGES.xlsx
+++ b/back-end/uploads/TEST 1 - ETS 2024/TEST 1 - ETS 2024-PASSAGES.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>section</t>
   </si>
   <si>
-    <t>listening</t>
-  </si>
-  <si>
     <t>reading</t>
   </si>
   <si>
@@ -42,145 +39,115 @@
     <t>images</t>
   </si>
   <si>
-    <t>passage62-64</t>
-  </si>
-  <si>
-    <t>62-64.png</t>
-  </si>
-  <si>
-    <t>passage65-67</t>
-  </si>
-  <si>
-    <t>65-67.png</t>
-  </si>
-  <si>
-    <t>passage68-70</t>
-  </si>
-  <si>
-    <t>68-70.png</t>
-  </si>
-  <si>
-    <t>passage95-97</t>
-  </si>
-  <si>
-    <t>95-97.png</t>
-  </si>
-  <si>
-    <t>passage98-100</t>
-  </si>
-  <si>
-    <t>98-100.png</t>
-  </si>
-  <si>
-    <t>passage131-134</t>
+    <t>passage-131-134</t>
   </si>
   <si>
     <t>131-134.png</t>
   </si>
   <si>
-    <t>passage135-138</t>
+    <t>passage-135-138</t>
   </si>
   <si>
     <t>135-138.png</t>
   </si>
   <si>
-    <t>passage139-142</t>
+    <t>passage-139-142</t>
   </si>
   <si>
     <t>139-142.png</t>
   </si>
   <si>
-    <t>passage143-146</t>
+    <t>passage-143-146</t>
   </si>
   <si>
     <t>143-146.png</t>
   </si>
   <si>
-    <t>passage147-148</t>
+    <t>passage-147-148</t>
   </si>
   <si>
     <t>147-148.png</t>
   </si>
   <si>
-    <t>passage149-150</t>
+    <t>passage-149-150</t>
   </si>
   <si>
     <t>149-150.png</t>
   </si>
   <si>
-    <t>passage151-152</t>
+    <t>passage-151-152</t>
   </si>
   <si>
     <t>151-152.png</t>
   </si>
   <si>
-    <t>passage153-154</t>
+    <t>passage-153-154</t>
   </si>
   <si>
     <t>153-154.png</t>
   </si>
   <si>
-    <t>passage155-157</t>
+    <t>passage-155-157</t>
   </si>
   <si>
     <t>155-157.png</t>
   </si>
   <si>
-    <t>passage158-160</t>
+    <t>passage-158-160</t>
   </si>
   <si>
     <t>158-160.png</t>
   </si>
   <si>
-    <t>passage161-164</t>
+    <t>passage-161-164</t>
   </si>
   <si>
     <t>161-164.png</t>
   </si>
   <si>
-    <t>passage165-167</t>
+    <t>passage-165-167</t>
   </si>
   <si>
     <t>165-167.png</t>
   </si>
   <si>
-    <t>passage168-171</t>
+    <t>passage-168-171</t>
   </si>
   <si>
     <t>168-171.png</t>
   </si>
   <si>
-    <t>passage172-175</t>
+    <t>passage-172-175</t>
   </si>
   <si>
     <t>172-175.png</t>
   </si>
   <si>
-    <t>passage176-180</t>
+    <t>passage-176-180</t>
   </si>
   <si>
     <t>176-180-1.png, 176-180-2.png</t>
   </si>
   <si>
-    <t>passage181-185</t>
+    <t>passage-181-185</t>
   </si>
   <si>
     <t>181-185-1.png, 181-185-2.png</t>
   </si>
   <si>
-    <t>passage186-190</t>
+    <t>passage-186-190</t>
   </si>
   <si>
     <t>186-190-1.png, 186-190-2.png, 186-190-3.png</t>
   </si>
   <si>
-    <t>passage191-195</t>
+    <t>passage-191-195</t>
   </si>
   <si>
     <t>191-195-1.png, 191-195-2.png, 191-195-3.png</t>
   </si>
   <si>
-    <t>passage196-200</t>
+    <t>passage-196-200</t>
   </si>
   <si>
     <t>196-200-1.png, 196-200-2.png, 196-200-3.png</t>
@@ -461,7 +428,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:E995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -478,16 +445,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -495,10 +462,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -506,10 +473,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -517,10 +484,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -528,10 +495,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -539,220 +506,180 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="B21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="B22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="B24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>54</v>
-      </c>
+      <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
@@ -3663,21 +3590,6 @@
     </row>
     <row r="995" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B995" s="1"/>
-    </row>
-    <row r="996" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B996" s="1"/>
-    </row>
-    <row r="997" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B997" s="1"/>
-    </row>
-    <row r="998" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B998" s="1"/>
-    </row>
-    <row r="999" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B999" s="1"/>
-    </row>
-    <row r="1000" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B1000" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
create user_answer featurem, return result user test answer, save in db
</commit_message>
<xml_diff>
--- a/back-end/uploads/TEST 1 - ETS 2024/TEST 1 - ETS 2024-PASSAGES.xlsx
+++ b/back-end/uploads/TEST 1 - ETS 2024/TEST 1 - ETS 2024-PASSAGES.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OS\Desktop\TEST1 - ETS2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -39,118 +39,118 @@
     <t>images</t>
   </si>
   <si>
-    <t>passage-131-134</t>
-  </si>
-  <si>
     <t>131-134.png</t>
   </si>
   <si>
-    <t>passage-135-138</t>
-  </si>
-  <si>
     <t>135-138.png</t>
   </si>
   <si>
-    <t>passage-139-142</t>
-  </si>
-  <si>
     <t>139-142.png</t>
   </si>
   <si>
-    <t>passage-143-146</t>
-  </si>
-  <si>
     <t>143-146.png</t>
   </si>
   <si>
-    <t>passage-147-148</t>
-  </si>
-  <si>
     <t>147-148.png</t>
   </si>
   <si>
-    <t>passage-149-150</t>
-  </si>
-  <si>
     <t>149-150.png</t>
   </si>
   <si>
-    <t>passage-151-152</t>
-  </si>
-  <si>
     <t>151-152.png</t>
   </si>
   <si>
-    <t>passage-153-154</t>
-  </si>
-  <si>
     <t>153-154.png</t>
   </si>
   <si>
-    <t>passage-155-157</t>
-  </si>
-  <si>
     <t>155-157.png</t>
   </si>
   <si>
-    <t>passage-158-160</t>
-  </si>
-  <si>
     <t>158-160.png</t>
   </si>
   <si>
-    <t>passage-161-164</t>
-  </si>
-  <si>
     <t>161-164.png</t>
   </si>
   <si>
-    <t>passage-165-167</t>
-  </si>
-  <si>
     <t>165-167.png</t>
   </si>
   <si>
-    <t>passage-168-171</t>
-  </si>
-  <si>
     <t>168-171.png</t>
   </si>
   <si>
-    <t>passage-172-175</t>
-  </si>
-  <si>
     <t>172-175.png</t>
   </si>
   <si>
-    <t>passage-176-180</t>
-  </si>
-  <si>
     <t>176-180-1.png, 176-180-2.png</t>
   </si>
   <si>
-    <t>passage-181-185</t>
-  </si>
-  <si>
     <t>181-185-1.png, 181-185-2.png</t>
   </si>
   <si>
-    <t>passage-186-190</t>
-  </si>
-  <si>
     <t>186-190-1.png, 186-190-2.png, 186-190-3.png</t>
   </si>
   <si>
-    <t>passage-191-195</t>
-  </si>
-  <si>
     <t>191-195-1.png, 191-195-2.png, 191-195-3.png</t>
   </si>
   <si>
-    <t>passage-196-200</t>
-  </si>
-  <si>
     <t>196-200-1.png, 196-200-2.png, 196-200-3.png</t>
+  </si>
+  <si>
+    <t>passage131-134</t>
+  </si>
+  <si>
+    <t>passage135-138</t>
+  </si>
+  <si>
+    <t>passage139-142</t>
+  </si>
+  <si>
+    <t>passage143-146</t>
+  </si>
+  <si>
+    <t>passage147-148</t>
+  </si>
+  <si>
+    <t>passage149-150</t>
+  </si>
+  <si>
+    <t>passage151-152</t>
+  </si>
+  <si>
+    <t>passage153-154</t>
+  </si>
+  <si>
+    <t>passage155-157</t>
+  </si>
+  <si>
+    <t>passage158-160</t>
+  </si>
+  <si>
+    <t>passage161-164</t>
+  </si>
+  <si>
+    <t>passage165-167</t>
+  </si>
+  <si>
+    <t>passage168-171</t>
+  </si>
+  <si>
+    <t>passage172-175</t>
+  </si>
+  <si>
+    <t>passage176-180</t>
+  </si>
+  <si>
+    <t>passage181-185</t>
+  </si>
+  <si>
+    <t>passage186-190</t>
+  </si>
+  <si>
+    <t>passage191-195</t>
+  </si>
+  <si>
+    <t>passage196-200</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,9 @@
   </sheetPr>
   <dimension ref="A1:E995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -457,261 +459,261 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
     </row>
     <row r="37" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>